<commit_message>
Added login page tests
</commit_message>
<xml_diff>
--- a/src/test/resources/OrangeHrmLoginPageTests.xlsx
+++ b/src/test/resources/OrangeHrmLoginPageTests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/GitHub/Selenium_PageObjectModel/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/eclipse-workspace/OrangeHrmProject/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4D1EA-5B70-9C46-86C4-E3958851D6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9356B6-ABC5-424C-BF55-CA07D17B953A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{3E7CED82-5598-444F-B316-A93909B7ED70}"/>
   </bookViews>
@@ -68,16 +68,16 @@
     <t>TC_04</t>
   </si>
   <si>
-    <t>validateLoginWithValidUserNameAndValidPassword</t>
-  </si>
-  <si>
-    <t>validateLoginWIthInValidUsernameAndvalidPassword</t>
-  </si>
-  <si>
-    <t>validateLoginWIthValidUsernameAndInvalidPassword</t>
-  </si>
-  <si>
-    <t>validateLoginWIthInValidUsernameAndInvalidPassword</t>
+    <t>validateLoginFeatureWithValidUserNameAndValidPassword</t>
+  </si>
+  <si>
+    <t>validateLoginFeatureWIthValidUsernameAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>validateLoginFeatureWIthInvalidUsernameAndInvalidPassword</t>
+  </si>
+  <si>
+    <t>validateLoginFeatureWIthInvalidUsernameAndValidPassword</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -519,7 +519,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -533,7 +533,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added Extent report script
</commit_message>
<xml_diff>
--- a/src/test/resources/OrangeHrmLoginPageTests.xlsx
+++ b/src/test/resources/OrangeHrmLoginPageTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/eclipse-workspace/OrangeHrmProject/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9356B6-ABC5-424C-BF55-CA07D17B953A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87BB76F-C2E5-6643-B223-A98F8CAE4FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{3E7CED82-5598-444F-B316-A93909B7ED70}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{3E7CED82-5598-444F-B316-A93909B7ED70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added take Screenshot code
</commit_message>
<xml_diff>
--- a/src/test/resources/OrangeHrmLoginPageTests.xlsx
+++ b/src/test/resources/OrangeHrmLoginPageTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/eclipse-workspace/OrangeHrmProject/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87BB76F-C2E5-6643-B223-A98F8CAE4FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1613C04-5922-1342-84E9-AE19DAA9D148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{3E7CED82-5598-444F-B316-A93909B7ED70}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>